<commit_message>
Update Aktiviteiten-voorbeeld.xlsx with rol column
</commit_message>
<xml_diff>
--- a/public/data/Aktiviteiten-voorbeeld.xlsx
+++ b/public/data/Aktiviteiten-voorbeeld.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkkbh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkkbh\Documents\Curso-ai\Def-apps\Fysio-Jaarplanning-docenten\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7ECDA179-58CB-4AF2-9053-386E9E0B5698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CE5D6F-0EE3-4D51-B69E-5DD0E0A11687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FF0CAB9B-7EA0-4AB2-8DC2-D7923B1D1BE5}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{FF0CAB9B-7EA0-4AB2-8DC2-D7923B1D1BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>Wat?</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Praktijkbureau</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>Studenten</t>
   </si>
 </sst>
 </file>
@@ -232,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -268,12 +274,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -330,6 +347,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="20" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -667,15 +687,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23938686-1923-49A3-9D51-E7888FD727EC}">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:V5"/>
+    <sheetView tabSelected="1" topLeftCell="G3" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2:W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -742,8 +762,11 @@
       <c r="V1" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="W1" s="20" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" ht="81.599999999999994" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -780,8 +803,11 @@
         <v>24</v>
       </c>
       <c r="V2" s="9"/>
+      <c r="W2" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" ht="51" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="51" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
@@ -820,8 +846,11 @@
       <c r="V3" s="9" t="s">
         <v>24</v>
       </c>
+      <c r="W3" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>27</v>
       </c>
@@ -852,8 +881,11 @@
       <c r="T4" s="9"/>
       <c r="U4" s="9"/>
       <c r="V4" s="9"/>
+      <c r="W4" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" ht="122.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="122.4" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>29</v>
       </c>
@@ -896,6 +928,9 @@
         <v>24</v>
       </c>
       <c r="V5" s="9"/>
+      <c r="W5" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>